<commit_message>
New decision_tree code after fixing graphviz via homebrew
</commit_message>
<xml_diff>
--- a/decision_tree/IG_sample.xlsx
+++ b/decision_tree/IG_sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PlayGolf" sheetId="1" r:id="rId1"/>
@@ -412,7 +412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -727,7 +727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>